<commit_message>
Normalise match classification for older workbooks
</commit_message>
<xml_diff>
--- a/Data/Workbooks/1_best_matches_set.xlsx
+++ b/Data/Workbooks/1_best_matches_set.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynko\Desktop\Thesis\Data\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F686FC-832F-48E3-ACDA-A9A7B9F1B59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F96FE1-F73B-4733-87C6-F79D04C48208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42750" yWindow="2445" windowWidth="21600" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="best_matches" sheetId="1" r:id="rId1"/>
@@ -242,48 +242,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,76 +271,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,166 +294,8 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -567,207 +303,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1081,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C211" sqref="C211"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,7 +760,7 @@
       <c r="E3">
         <v>414</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G3">
@@ -1248,7 +801,7 @@
       <c r="B4">
         <v>412</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D4">
@@ -1257,7 +810,7 @@
       <c r="E4">
         <v>701</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G4">
@@ -1607,7 +1160,7 @@
       <c r="E11">
         <v>303</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G11">
@@ -1657,7 +1210,7 @@
       <c r="E12">
         <v>607</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G12">
@@ -1757,7 +1310,7 @@
       <c r="E14">
         <v>706</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G14">
@@ -1848,7 +1401,7 @@
       <c r="B16">
         <v>108</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D16">
@@ -1957,7 +1510,7 @@
       <c r="E18">
         <v>604</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G18">
@@ -1998,7 +1551,7 @@
       <c r="B19">
         <v>415</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D19">
@@ -2007,7 +1560,7 @@
       <c r="E19">
         <v>301</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G19">
@@ -2057,7 +1610,7 @@
       <c r="E20">
         <v>303</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G20">
@@ -2698,7 +2251,7 @@
       <c r="B33">
         <v>414</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D33">
@@ -2748,7 +2301,7 @@
       <c r="B34">
         <v>507</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D34">
@@ -2798,7 +2351,7 @@
       <c r="B35">
         <v>507</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D35">
@@ -2848,7 +2401,7 @@
       <c r="B36">
         <v>504</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D36">
@@ -2857,7 +2410,7 @@
       <c r="E36">
         <v>505</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G36">
@@ -2957,7 +2510,7 @@
       <c r="E38">
         <v>305</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G38">
@@ -3007,7 +2560,7 @@
       <c r="E39">
         <v>405</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G39">
@@ -3048,7 +2601,7 @@
       <c r="B40">
         <v>413</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D40">
@@ -3107,7 +2660,7 @@
       <c r="E41">
         <v>412</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G41">
@@ -3407,7 +2960,7 @@
       <c r="E47">
         <v>412</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G47">
@@ -3498,7 +3051,7 @@
       <c r="B49">
         <v>411</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D49">
@@ -3657,7 +3210,7 @@
       <c r="E52">
         <v>412</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G52">
@@ -3698,7 +3251,7 @@
       <c r="B53">
         <v>504</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D53">
@@ -3748,7 +3301,7 @@
       <c r="B54">
         <v>701</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D54">
@@ -3857,7 +3410,7 @@
       <c r="E56">
         <v>305</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G56">
@@ -4148,7 +3701,7 @@
       <c r="B62">
         <v>411</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D62">
@@ -4307,7 +3860,7 @@
       <c r="E65">
         <v>305</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="3" t="s">
         <v>18</v>
       </c>
       <c r="G65">
@@ -4407,7 +3960,7 @@
       <c r="E67">
         <v>416</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G67">
@@ -4457,7 +4010,7 @@
       <c r="E68">
         <v>416</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G68">
@@ -4507,7 +4060,7 @@
       <c r="E69">
         <v>416</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G69">
@@ -4557,7 +4110,7 @@
       <c r="E70">
         <v>416</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G70">
@@ -4607,7 +4160,7 @@
       <c r="E71">
         <v>416</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="3" t="s">
         <v>37</v>
       </c>
       <c r="G71">
@@ -4757,7 +4310,7 @@
       <c r="E74">
         <v>411</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G74">
@@ -4998,7 +4551,7 @@
       <c r="B79">
         <v>501</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D79">
@@ -5307,7 +4860,7 @@
       <c r="E85">
         <v>109</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="F85" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G85">
@@ -5357,7 +4910,7 @@
       <c r="E86">
         <v>302</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="F86" s="2" t="s">
         <v>45</v>
       </c>
       <c r="G86">
@@ -5398,7 +4951,7 @@
       <c r="B87">
         <v>502</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D87">
@@ -5807,7 +5360,7 @@
       <c r="E95">
         <v>701</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F95" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G95">
@@ -5848,7 +5401,7 @@
       <c r="B96">
         <v>608</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D96">
@@ -6007,7 +5560,7 @@
       <c r="E99">
         <v>302</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G99">
@@ -6048,7 +5601,7 @@
       <c r="B100">
         <v>302</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D100">
@@ -6157,7 +5710,7 @@
       <c r="E102">
         <v>504</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="F102" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G102">
@@ -6207,7 +5760,7 @@
       <c r="E103">
         <v>604</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F103" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G103">
@@ -6448,7 +6001,7 @@
       <c r="B108">
         <v>404</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D108">
@@ -6548,7 +6101,7 @@
       <c r="B110">
         <v>412</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C110" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D110">
@@ -6848,7 +6401,7 @@
       <c r="B116">
         <v>109</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C116" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D116">
@@ -6948,7 +6501,7 @@
       <c r="B118">
         <v>504</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D118">
@@ -6957,7 +6510,7 @@
       <c r="E118">
         <v>409</v>
       </c>
-      <c r="F118" s="3" t="s">
+      <c r="F118" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G118">
@@ -6998,7 +6551,7 @@
       <c r="B119">
         <v>416</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D119">
@@ -7057,7 +6610,7 @@
       <c r="E120">
         <v>409</v>
       </c>
-      <c r="F120" s="3" t="s">
+      <c r="F120" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G120">
@@ -7098,7 +6651,7 @@
       <c r="B121">
         <v>105</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D121">
@@ -7148,7 +6701,7 @@
       <c r="B122">
         <v>705</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D122">
@@ -7357,7 +6910,7 @@
       <c r="E126">
         <v>412</v>
       </c>
-      <c r="F126" s="1" t="s">
+      <c r="F126" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G126">
@@ -7498,7 +7051,7 @@
       <c r="B129">
         <v>403</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D129">
@@ -7507,7 +7060,7 @@
       <c r="E129">
         <v>414</v>
       </c>
-      <c r="F129" s="3" t="s">
+      <c r="F129" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G129">
@@ -7598,7 +7151,7 @@
       <c r="B131">
         <v>401</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D131">
@@ -7698,7 +7251,7 @@
       <c r="B133">
         <v>403</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D133">
@@ -7798,7 +7351,7 @@
       <c r="B135">
         <v>501</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="C135" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D135">
@@ -7848,7 +7401,7 @@
       <c r="B136">
         <v>404</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D136">
@@ -8007,7 +7560,7 @@
       <c r="E139">
         <v>411</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="F139" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G139">
@@ -8207,7 +7760,7 @@
       <c r="E143">
         <v>103</v>
       </c>
-      <c r="F143" s="3" t="s">
+      <c r="F143" s="2" t="s">
         <v>56</v>
       </c>
       <c r="G143">
@@ -8498,7 +8051,7 @@
       <c r="B149">
         <v>413</v>
       </c>
-      <c r="C149" s="2" t="s">
+      <c r="C149" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D149">
@@ -8707,7 +8260,7 @@
       <c r="E153">
         <v>704</v>
       </c>
-      <c r="F153" s="2" t="s">
+      <c r="F153" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G153">
@@ -8757,7 +8310,7 @@
       <c r="E154">
         <v>103</v>
       </c>
-      <c r="F154" s="2" t="s">
+      <c r="F154" s="3" t="s">
         <v>56</v>
       </c>
       <c r="G154">
@@ -9007,7 +8560,7 @@
       <c r="E159">
         <v>701</v>
       </c>
-      <c r="F159" s="2" t="s">
+      <c r="F159" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G159">
@@ -9207,7 +8760,7 @@
       <c r="E163">
         <v>303</v>
       </c>
-      <c r="F163" s="2" t="s">
+      <c r="F163" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G163">
@@ -9857,7 +9410,7 @@
       <c r="E176">
         <v>404</v>
       </c>
-      <c r="F176" s="3" t="s">
+      <c r="F176" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G176">
@@ -10007,7 +9560,7 @@
       <c r="E179">
         <v>202</v>
       </c>
-      <c r="F179" s="3" t="s">
+      <c r="F179" s="1" t="s">
         <v>70</v>
       </c>
       <c r="G179">
@@ -10257,7 +9810,7 @@
       <c r="E184">
         <v>605</v>
       </c>
-      <c r="F184" s="3" t="s">
+      <c r="F184" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G184">
@@ -10348,7 +9901,7 @@
       <c r="B186">
         <v>107</v>
       </c>
-      <c r="C186" s="3" t="s">
+      <c r="C186" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D186">
@@ -10357,7 +9910,7 @@
       <c r="E186">
         <v>109</v>
       </c>
-      <c r="F186" s="3" t="s">
+      <c r="F186" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G186">
@@ -10407,7 +9960,7 @@
       <c r="E187">
         <v>101</v>
       </c>
-      <c r="F187" s="1" t="s">
+      <c r="F187" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G187">
@@ -10498,7 +10051,7 @@
       <c r="B189">
         <v>302</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D189">
@@ -10507,7 +10060,7 @@
       <c r="E189">
         <v>305</v>
       </c>
-      <c r="F189" s="3" t="s">
+      <c r="F189" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G189">
@@ -10598,7 +10151,7 @@
       <c r="B191">
         <v>302</v>
       </c>
-      <c r="C191" s="2" t="s">
+      <c r="C191" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D191">
@@ -10657,7 +10210,7 @@
       <c r="E192">
         <v>704</v>
       </c>
-      <c r="F192" s="2" t="s">
+      <c r="F192" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G192">
@@ -10757,7 +10310,7 @@
       <c r="E194">
         <v>102</v>
       </c>
-      <c r="F194" s="2" t="s">
+      <c r="F194" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G194">
@@ -10779,7 +10332,7 @@
         <v>66</v>
       </c>
       <c r="M194">
-        <v>1.2737486838182699</v>
+        <v>1.2737486838182701</v>
       </c>
       <c r="N194">
         <v>702</v>
@@ -10907,7 +10460,7 @@
       <c r="E197">
         <v>404</v>
       </c>
-      <c r="F197" s="3" t="s">
+      <c r="F197" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G197">
@@ -11098,7 +10651,7 @@
       <c r="B201">
         <v>302</v>
       </c>
-      <c r="C201" s="2" t="s">
+      <c r="C201" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D201">
@@ -11107,7 +10660,7 @@
       <c r="E201">
         <v>304</v>
       </c>
-      <c r="F201" s="3" t="s">
+      <c r="F201" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G201">
@@ -11157,7 +10710,7 @@
       <c r="E202">
         <v>404</v>
       </c>
-      <c r="F202" s="3" t="s">
+      <c r="F202" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G202">
@@ -11207,7 +10760,7 @@
       <c r="E203">
         <v>302</v>
       </c>
-      <c r="F203" s="1" t="s">
+      <c r="F203" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G203">
@@ -11257,7 +10810,7 @@
       <c r="E204">
         <v>412</v>
       </c>
-      <c r="F204" s="3" t="s">
+      <c r="F204" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G204">
@@ -11348,7 +10901,7 @@
       <c r="B206">
         <v>302</v>
       </c>
-      <c r="C206" s="2" t="s">
+      <c r="C206" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D206">
@@ -11357,7 +10910,7 @@
       <c r="E206">
         <v>404</v>
       </c>
-      <c r="F206" s="3" t="s">
+      <c r="F206" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G206">
@@ -11507,7 +11060,7 @@
       <c r="E209">
         <v>402</v>
       </c>
-      <c r="F209" s="2" t="s">
+      <c r="F209" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G209">
@@ -11557,7 +11110,7 @@
       <c r="E210">
         <v>502</v>
       </c>
-      <c r="F210" s="1" t="s">
+      <c r="F210" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G210">
@@ -11598,7 +11151,7 @@
       <c r="B211">
         <v>201</v>
       </c>
-      <c r="C211" s="2" t="s">
+      <c r="C211" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D211">
@@ -11648,7 +11201,7 @@
       <c r="B212">
         <v>203</v>
       </c>
-      <c r="C212" s="3" t="s">
+      <c r="C212" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D212">
@@ -11707,7 +11260,7 @@
       <c r="E213">
         <v>203</v>
       </c>
-      <c r="F213" s="3" t="s">
+      <c r="F213" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G213">

</xml_diff>